<commit_message>
Update Quinn's name in data/ and data-raw/ files that reference players names.
</commit_message>
<xml_diff>
--- a/data-raw/fieldplayers_overall_season_2018.xlsx
+++ b/data-raw/fieldplayers_overall_season_2018.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27417"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sophiatannir/Documents/nwslR/data-raw/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aliso\Desktop\nwslR\data-raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA4C17B-6D8C-4731-B270-CCBA3ACAB61F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8800" yWindow="5980" windowWidth="25600" windowHeight="14320" tabRatio="500"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -626,9 +627,6 @@
     <t>Margaret Purce</t>
   </si>
   <si>
-    <t>Rebecca Quinn</t>
-  </si>
-  <si>
     <t>Megan Rapinoe</t>
   </si>
   <si>
@@ -810,12 +808,15 @@
   </si>
   <si>
     <t>Gunnhildur Yrsa Jónsdóttir</t>
+  </si>
+  <si>
+    <t>Quinn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -873,6 +874,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1140,14 +1144,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P213"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A209" workbookViewId="0">
-      <selection activeCell="B211" sqref="B211"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="B161" sqref="B161"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.33203125" bestFit="1" customWidth="1"/>
@@ -1177,7 +1181,7 @@
     <col min="30" max="30" width="8.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1227,7 +1231,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1277,7 +1281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1327,7 +1331,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1377,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1427,7 +1431,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1477,7 +1481,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1527,7 +1531,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1577,12 +1581,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>35</v>
@@ -1627,7 +1631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1677,7 +1681,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1727,7 +1731,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1777,7 +1781,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1827,7 +1831,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1877,7 +1881,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1927,7 +1931,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1973,7 +1977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2023,7 +2027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2073,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2123,7 +2127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2173,7 +2177,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2223,7 +2227,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2271,7 +2275,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2321,7 +2325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2371,7 +2375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2421,7 +2425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2471,7 +2475,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2521,7 +2525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2571,7 +2575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2621,7 +2625,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2671,7 +2675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2721,7 +2725,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2771,7 +2775,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>32</v>
       </c>
@@ -2821,7 +2825,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>33</v>
       </c>
@@ -2871,7 +2875,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>34</v>
       </c>
@@ -2921,12 +2925,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>35</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>71</v>
@@ -2971,7 +2975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>36</v>
       </c>
@@ -3019,7 +3023,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>37</v>
       </c>
@@ -3069,7 +3073,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -3119,7 +3123,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -3169,7 +3173,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -3219,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -3269,7 +3273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -3319,7 +3323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>43</v>
       </c>
@@ -3369,7 +3373,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>44</v>
       </c>
@@ -3415,7 +3419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>45</v>
       </c>
@@ -3465,7 +3469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>46</v>
       </c>
@@ -3515,7 +3519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>47</v>
       </c>
@@ -3565,7 +3569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>48</v>
       </c>
@@ -3615,7 +3619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>49</v>
       </c>
@@ -3665,7 +3669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A51" s="1">
         <v>50</v>
       </c>
@@ -3715,7 +3719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>51</v>
       </c>
@@ -3765,7 +3769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>52</v>
       </c>
@@ -3815,7 +3819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>53</v>
       </c>
@@ -3865,7 +3869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>54</v>
       </c>
@@ -3915,7 +3919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>55</v>
       </c>
@@ -3965,7 +3969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>56</v>
       </c>
@@ -4015,7 +4019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>57</v>
       </c>
@@ -4065,7 +4069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>58</v>
       </c>
@@ -4115,7 +4119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>59</v>
       </c>
@@ -4165,7 +4169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>60</v>
       </c>
@@ -4215,7 +4219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>61</v>
       </c>
@@ -4265,7 +4269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>62</v>
       </c>
@@ -4315,7 +4319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>63</v>
       </c>
@@ -4365,7 +4369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>64</v>
       </c>
@@ -4415,7 +4419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>65</v>
       </c>
@@ -4465,7 +4469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>66</v>
       </c>
@@ -4515,7 +4519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>67</v>
       </c>
@@ -4565,7 +4569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>68</v>
       </c>
@@ -4615,7 +4619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>69</v>
       </c>
@@ -4665,7 +4669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>70</v>
       </c>
@@ -4715,7 +4719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>71</v>
       </c>
@@ -4765,7 +4769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>72</v>
       </c>
@@ -4815,7 +4819,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>73</v>
       </c>
@@ -4865,7 +4869,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>74</v>
       </c>
@@ -4915,7 +4919,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>75</v>
       </c>
@@ -4965,7 +4969,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>76</v>
       </c>
@@ -5015,7 +5019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>77</v>
       </c>
@@ -5065,7 +5069,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>78</v>
       </c>
@@ -5115,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>79</v>
       </c>
@@ -5165,7 +5169,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>80</v>
       </c>
@@ -5215,7 +5219,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>81</v>
       </c>
@@ -5265,7 +5269,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>82</v>
       </c>
@@ -5315,7 +5319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>83</v>
       </c>
@@ -5365,7 +5369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>84</v>
       </c>
@@ -5415,7 +5419,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>85</v>
       </c>
@@ -5465,7 +5469,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>86</v>
       </c>
@@ -5515,7 +5519,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>87</v>
       </c>
@@ -5565,7 +5569,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>88</v>
       </c>
@@ -5615,7 +5619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>89</v>
       </c>
@@ -5665,7 +5669,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>90</v>
       </c>
@@ -5715,7 +5719,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>91</v>
       </c>
@@ -5765,7 +5769,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>92</v>
       </c>
@@ -5813,7 +5817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>93</v>
       </c>
@@ -5863,7 +5867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>94</v>
       </c>
@@ -5913,7 +5917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>95</v>
       </c>
@@ -5963,7 +5967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A97" s="1">
         <v>96</v>
       </c>
@@ -6013,7 +6017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A98" s="1">
         <v>97</v>
       </c>
@@ -6063,7 +6067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A99" s="1">
         <v>98</v>
       </c>
@@ -6113,7 +6117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A100" s="1">
         <v>99</v>
       </c>
@@ -6163,7 +6167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A101" s="1">
         <v>100</v>
       </c>
@@ -6213,7 +6217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A102" s="1">
         <v>101</v>
       </c>
@@ -6263,7 +6267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A103" s="1">
         <v>102</v>
       </c>
@@ -6313,7 +6317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A104" s="1">
         <v>103</v>
       </c>
@@ -6363,7 +6367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A105" s="1">
         <v>104</v>
       </c>
@@ -6413,7 +6417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A106" s="1">
         <v>105</v>
       </c>
@@ -6463,7 +6467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A107" s="1">
         <v>106</v>
       </c>
@@ -6513,7 +6517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A108" s="1">
         <v>107</v>
       </c>
@@ -6563,7 +6567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A109" s="1">
         <v>108</v>
       </c>
@@ -6613,7 +6617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A110" s="1">
         <v>109</v>
       </c>
@@ -6663,7 +6667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A111" s="1">
         <v>110</v>
       </c>
@@ -6713,7 +6717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A112" s="1">
         <v>111</v>
       </c>
@@ -6763,7 +6767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A113" s="1">
         <v>112</v>
       </c>
@@ -6813,7 +6817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A114" s="1">
         <v>113</v>
       </c>
@@ -6863,7 +6867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A115" s="1">
         <v>114</v>
       </c>
@@ -6913,7 +6917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A116" s="1">
         <v>115</v>
       </c>
@@ -6963,7 +6967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A117" s="1">
         <v>116</v>
       </c>
@@ -7013,7 +7017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A118" s="1">
         <v>117</v>
       </c>
@@ -7063,7 +7067,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A119" s="1">
         <v>118</v>
       </c>
@@ -7113,7 +7117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A120" s="1">
         <v>119</v>
       </c>
@@ -7163,7 +7167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A121" s="1">
         <v>120</v>
       </c>
@@ -7213,7 +7217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A122" s="1">
         <v>121</v>
       </c>
@@ -7263,7 +7267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A123" s="1">
         <v>122</v>
       </c>
@@ -7313,7 +7317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A124" s="1">
         <v>123</v>
       </c>
@@ -7363,7 +7367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A125" s="1">
         <v>124</v>
       </c>
@@ -7413,7 +7417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="126" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A126" s="1">
         <v>125</v>
       </c>
@@ -7463,7 +7467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="127" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A127" s="1">
         <v>126</v>
       </c>
@@ -7513,7 +7517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A128" s="1">
         <v>127</v>
       </c>
@@ -7563,7 +7567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A129" s="1">
         <v>128</v>
       </c>
@@ -7613,7 +7617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A130" s="1">
         <v>129</v>
       </c>
@@ -7663,7 +7667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A131" s="1">
         <v>130</v>
       </c>
@@ -7713,12 +7717,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A132" s="1">
         <v>131</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C132" s="2" t="s">
         <v>27</v>
@@ -7763,7 +7767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A133" s="1">
         <v>132</v>
       </c>
@@ -7813,7 +7817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A134" s="1">
         <v>133</v>
       </c>
@@ -7863,7 +7867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A135" s="1">
         <v>134</v>
       </c>
@@ -7913,7 +7917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A136" s="1">
         <v>135</v>
       </c>
@@ -7963,7 +7967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A137" s="1">
         <v>136</v>
       </c>
@@ -8013,12 +8017,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A138" s="1">
         <v>137</v>
       </c>
       <c r="B138" s="2" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C138" s="2" t="s">
         <v>133</v>
@@ -8063,7 +8067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A139" s="1">
         <v>138</v>
       </c>
@@ -8113,7 +8117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A140" s="1">
         <v>139</v>
       </c>
@@ -8163,7 +8167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A141" s="1">
         <v>140</v>
       </c>
@@ -8213,7 +8217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A142" s="1">
         <v>141</v>
       </c>
@@ -8263,7 +8267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A143" s="1">
         <v>142</v>
       </c>
@@ -8313,7 +8317,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A144" s="1">
         <v>143</v>
       </c>
@@ -8363,7 +8367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A145" s="1">
         <v>144</v>
       </c>
@@ -8413,7 +8417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A146" s="1">
         <v>145</v>
       </c>
@@ -8463,7 +8467,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="147" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A147" s="1">
         <v>146</v>
       </c>
@@ -8513,7 +8517,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="148" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A148" s="1">
         <v>147</v>
       </c>
@@ -8563,7 +8567,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="149" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A149" s="1">
         <v>148</v>
       </c>
@@ -8613,7 +8617,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="150" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A150" s="1">
         <v>149</v>
       </c>
@@ -8663,7 +8667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="151" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A151" s="1">
         <v>150</v>
       </c>
@@ -8713,7 +8717,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="152" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A152" s="1">
         <v>151</v>
       </c>
@@ -8763,7 +8767,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="153" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A153" s="1">
         <v>152</v>
       </c>
@@ -8813,7 +8817,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="154" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A154" s="1">
         <v>153</v>
       </c>
@@ -8863,7 +8867,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="155" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A155" s="1">
         <v>154</v>
       </c>
@@ -8913,7 +8917,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="156" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A156" s="1">
         <v>155</v>
       </c>
@@ -8963,7 +8967,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="157" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A157" s="1">
         <v>156</v>
       </c>
@@ -9013,7 +9017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="158" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -9063,7 +9067,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -9113,12 +9117,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A160" s="1">
         <v>159</v>
       </c>
       <c r="B160" s="2" t="s">
-        <v>199</v>
+        <v>260</v>
       </c>
       <c r="C160" s="2" t="s">
         <v>24</v>
@@ -9163,12 +9167,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A161" s="1">
         <v>160</v>
       </c>
       <c r="B161" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C161" s="2" t="s">
         <v>31</v>
@@ -9213,12 +9217,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A162" s="1">
         <v>161</v>
       </c>
       <c r="B162" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C162" s="2" t="s">
         <v>60</v>
@@ -9263,12 +9267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A163" s="1">
         <v>162</v>
       </c>
       <c r="B163" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C163" s="2" t="s">
         <v>31</v>
@@ -9313,12 +9317,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A164" s="1">
         <v>163</v>
       </c>
       <c r="B164" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="C164" s="2" t="s">
         <v>31</v>
@@ -9363,12 +9367,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A165" s="1">
         <v>164</v>
       </c>
       <c r="B165" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C165" s="2" t="s">
         <v>31</v>
@@ -9413,12 +9417,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A166" s="1">
         <v>165</v>
       </c>
       <c r="B166" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C166" s="2" t="s">
         <v>31</v>
@@ -9463,12 +9467,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A167" s="1">
         <v>166</v>
       </c>
       <c r="B167" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C167" s="2" t="s">
         <v>31</v>
@@ -9513,15 +9517,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A168" s="1">
         <v>167</v>
       </c>
       <c r="B168" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C168" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D168" s="2" t="s">
         <v>18</v>
@@ -9563,12 +9567,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A169" s="1">
         <v>168</v>
       </c>
       <c r="B169" s="2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C169" s="2" t="s">
         <v>31</v>
@@ -9613,12 +9617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A170" s="1">
         <v>169</v>
       </c>
       <c r="B170" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C170" s="2" t="s">
         <v>31</v>
@@ -9663,12 +9667,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A171" s="1">
         <v>170</v>
       </c>
       <c r="B171" s="2" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C171" s="2" t="s">
         <v>31</v>
@@ -9713,12 +9717,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A172" s="1">
         <v>171</v>
       </c>
       <c r="B172" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C172" s="2" t="s">
         <v>24</v>
@@ -9763,12 +9767,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A173" s="1">
         <v>172</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C173" s="2" t="s">
         <v>24</v>
@@ -9813,12 +9817,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A174" s="1">
         <v>173</v>
       </c>
       <c r="B174" s="2" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C174" s="2" t="s">
         <v>31</v>
@@ -9863,12 +9867,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A175" s="1">
         <v>174</v>
       </c>
       <c r="B175" s="2" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="C175" s="2" t="s">
         <v>31</v>
@@ -9913,12 +9917,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A176" s="1">
         <v>175</v>
       </c>
       <c r="B176" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C176" s="2" t="s">
         <v>31</v>
@@ -9963,12 +9967,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="177" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A177" s="1">
         <v>176</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C177" s="2" t="s">
         <v>60</v>
@@ -10013,12 +10017,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="178" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A178" s="1">
         <v>177</v>
       </c>
       <c r="B178" s="2" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="C178" s="2" t="s">
         <v>24</v>
@@ -10063,12 +10067,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="179" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A179" s="1">
         <v>178</v>
       </c>
       <c r="B179" s="2" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C179" s="2" t="s">
         <v>31</v>
@@ -10113,12 +10117,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="180" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A180" s="1">
         <v>179</v>
       </c>
       <c r="B180" s="2" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C180" s="2" t="s">
         <v>31</v>
@@ -10163,12 +10167,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="181" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A181" s="1">
         <v>180</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C181" s="2" t="s">
         <v>31</v>
@@ -10213,15 +10217,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="182" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A182" s="1">
         <v>181</v>
       </c>
       <c r="B182" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="C182" s="2" t="s">
         <v>221</v>
-      </c>
-      <c r="C182" s="2" t="s">
-        <v>222</v>
       </c>
       <c r="D182" s="2" t="s">
         <v>28</v>
@@ -10263,12 +10267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="183" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A183" s="1">
         <v>182</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C183" s="2" t="s">
         <v>31</v>
@@ -10313,12 +10317,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="184" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A184" s="1">
         <v>183</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C184" s="2" t="s">
         <v>31</v>
@@ -10363,12 +10367,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="185" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A185" s="1">
         <v>184</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C185" s="2" t="s">
         <v>31</v>
@@ -10413,12 +10417,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="186" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A186" s="1">
         <v>185</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="C186" s="2" t="s">
         <v>31</v>
@@ -10463,12 +10467,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="187" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A187" s="1">
         <v>186</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C187" s="2" t="s">
         <v>31</v>
@@ -10513,12 +10517,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="188" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A188" s="1">
         <v>187</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C188" s="2" t="s">
         <v>49</v>
@@ -10563,12 +10567,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="189" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A189" s="1">
         <v>188</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C189" s="2" t="s">
         <v>31</v>
@@ -10613,12 +10617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="190" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A190" s="1">
         <v>189</v>
       </c>
       <c r="B190" s="2" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C190" s="2" t="s">
         <v>79</v>
@@ -10663,12 +10667,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="191" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A191" s="1">
         <v>190</v>
       </c>
       <c r="B191" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C191" s="2" t="s">
         <v>27</v>
@@ -10713,15 +10717,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="192" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A192" s="1">
         <v>191</v>
       </c>
       <c r="B192" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="C192" s="2" t="s">
         <v>232</v>
-      </c>
-      <c r="C192" s="2" t="s">
-        <v>233</v>
       </c>
       <c r="D192" s="2" t="s">
         <v>18</v>
@@ -10763,12 +10767,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A193" s="1">
         <v>192</v>
       </c>
       <c r="B193" s="2" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C193" s="2" t="s">
         <v>31</v>
@@ -10813,12 +10817,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A194" s="1">
         <v>193</v>
       </c>
       <c r="B194" s="2" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C194" s="2" t="s">
         <v>31</v>
@@ -10863,12 +10867,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A195" s="1">
         <v>194</v>
       </c>
       <c r="B195" s="2" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C195" s="2" t="s">
         <v>31</v>
@@ -10913,12 +10917,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A196" s="1">
         <v>195</v>
       </c>
       <c r="B196" s="2" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C196" s="2" t="s">
         <v>133</v>
@@ -10963,12 +10967,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A197" s="1">
         <v>196</v>
       </c>
       <c r="B197" s="2" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C197" s="2" t="s">
         <v>31</v>
@@ -11013,12 +11017,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A198" s="1">
         <v>197</v>
       </c>
       <c r="B198" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C198" s="2" t="s">
         <v>31</v>
@@ -11063,12 +11067,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A199" s="1">
         <v>198</v>
       </c>
       <c r="B199" s="2" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C199" s="2" t="s">
         <v>31</v>
@@ -11113,12 +11117,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A200" s="1">
         <v>199</v>
       </c>
       <c r="B200" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C200" s="2" t="s">
         <v>31</v>
@@ -11163,12 +11167,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A201" s="1">
         <v>200</v>
       </c>
       <c r="B201" s="2" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>31</v>
@@ -11213,12 +11217,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A202" s="1">
         <v>201</v>
       </c>
       <c r="B202" s="2" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C202" s="2" t="s">
         <v>49</v>
@@ -11263,12 +11267,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A203" s="1">
         <v>202</v>
       </c>
       <c r="B203" s="2" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C203" s="2" t="s">
         <v>60</v>
@@ -11313,12 +11317,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A204" s="1">
         <v>203</v>
       </c>
       <c r="B204" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C204" s="2" t="s">
         <v>31</v>
@@ -11363,12 +11367,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A205" s="1">
         <v>204</v>
       </c>
       <c r="B205" s="2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C205" s="2" t="s">
         <v>31</v>
@@ -11413,12 +11417,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A206" s="1">
         <v>205</v>
       </c>
       <c r="B206" s="2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C206" s="2" t="s">
         <v>31</v>
@@ -11463,12 +11467,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A207" s="1">
         <v>206</v>
       </c>
       <c r="B207" s="2" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C207" s="2" t="s">
         <v>139</v>
@@ -11513,12 +11517,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A208" s="1">
         <v>207</v>
       </c>
       <c r="B208" s="2" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C208" s="2" t="s">
         <v>31</v>
@@ -11563,12 +11567,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="209" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A209" s="1">
         <v>208</v>
       </c>
       <c r="B209" s="2" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C209" s="2" t="s">
         <v>31</v>
@@ -11613,12 +11617,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="210" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A210" s="1">
         <v>209</v>
       </c>
       <c r="B210" s="2" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C210" s="2" t="s">
         <v>31</v>
@@ -11663,15 +11667,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="211" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A211" s="1">
         <v>210</v>
       </c>
       <c r="B211" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C211" s="2" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D211" s="2" t="s">
         <v>28</v>
@@ -11713,12 +11717,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="212" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A212" s="1">
         <v>211</v>
       </c>
       <c r="B212" s="2" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C212" s="2" t="s">
         <v>24</v>
@@ -11763,12 +11767,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="213" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A213" s="1">
         <v>212</v>
       </c>
       <c r="B213" s="2" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C213" s="2" t="s">
         <v>31</v>

</xml_diff>